<commit_message>
Added a python script to collect the data into excel file
</commit_message>
<xml_diff>
--- a/paper/experiments.xlsx
+++ b/paper/experiments.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gk_pliki\uczelnia\doktorat\performance_modelling\repo\MMM\carma_cscs\CARMA\paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kabicm/Projects/carma-now/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E4C9E3CA-B977-3B4B-B8B0-A9618F3BEF19}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -354,6 +355,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -373,9 +377,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -657,22 +658,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AV33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AI3" sqref="AI3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="6.21875" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="14" width="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.109375" customWidth="1"/>
-    <col min="16" max="16" width="6.21875" customWidth="1"/>
+    <col min="15" max="16" width="6.1640625" customWidth="1"/>
     <col min="17" max="20" width="6" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="6" bestFit="1" customWidth="1"/>
@@ -683,7 +683,7 @@
     <col min="55" max="55" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:48" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:48" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O2" t="s">
         <v>12</v>
       </c>
@@ -691,7 +691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:48" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O3" t="s">
         <v>13</v>
       </c>
@@ -699,7 +699,7 @@
         <v>8847360</v>
       </c>
     </row>
-    <row r="4" spans="1:48" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:48" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
       <c r="C4" s="10"/>
       <c r="D4" s="11" t="s">
@@ -752,7 +752,7 @@
       <c r="AU4" s="12"/>
       <c r="AV4" s="12"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="23"/>
       <c r="B5" s="24"/>
       <c r="C5" s="2"/>
@@ -814,8 +814,8 @@
       <c r="AU5" s="3"/>
       <c r="AV5" s="3"/>
     </row>
-    <row r="6" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="45" t="s">
+    <row r="6" spans="1:48" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="24"/>
@@ -898,8 +898,8 @@
       </c>
       <c r="AV6" s="3"/>
     </row>
-    <row r="7" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="45"/>
+    <row r="7" spans="1:48" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
       <c r="B7" s="24"/>
       <c r="C7" s="16" t="s">
         <v>2</v>
@@ -1052,8 +1052,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A8" s="45"/>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A8" s="38"/>
       <c r="B8" s="24"/>
       <c r="C8" s="2" t="s">
         <v>3</v>
@@ -1106,8 +1106,8 @@
       <c r="AU8" s="19"/>
       <c r="AV8" s="19"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A9" s="45"/>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A9" s="38"/>
       <c r="B9" s="24"/>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -1160,8 +1160,8 @@
       <c r="AU9" s="8"/>
       <c r="AV9" s="8"/>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A10" s="38"/>
       <c r="B10" s="24"/>
       <c r="C10" s="2" t="s">
         <v>4</v>
@@ -1214,8 +1214,8 @@
       <c r="AU10" s="8"/>
       <c r="AV10" s="8"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A11" s="45"/>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A11" s="38"/>
       <c r="B11" s="24"/>
       <c r="C11" s="2" t="s">
         <v>6</v>
@@ -1268,7 +1268,7 @@
       <c r="AU11" s="8"/>
       <c r="AV11" s="8"/>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A12" s="25"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1318,7 +1318,7 @@
       <c r="AU12" s="5"/>
       <c r="AV12" s="5"/>
     </row>
-    <row r="13" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26"/>
       <c r="B13" s="27"/>
       <c r="C13" s="4"/>
@@ -1344,7 +1344,7 @@
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
-      <c r="Z13" s="38" t="s">
+      <c r="Z13" s="39" t="s">
         <v>14</v>
       </c>
       <c r="AA13" s="5" t="s">
@@ -1435,22 +1435,22 @@
         <v>5993</v>
       </c>
     </row>
-    <row r="14" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="40" t="s">
+    <row r="14" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="44" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" ref="D14:X14" si="10">FLOOR(SQRT(D7*$U$3/2),1)</f>
+        <f>FLOOR(SQRT(D7*$U$3/2),1)</f>
         <v>4206</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="D14:X14" si="10">FLOOR(SQRT(E7*$U$3/2),1)</f>
         <v>5564</v>
       </c>
       <c r="F14" s="4">
@@ -1530,7 +1530,7 @@
         <v>51519</v>
       </c>
       <c r="Y14" s="4"/>
-      <c r="Z14" s="38"/>
+      <c r="Z14" s="39"/>
       <c r="AA14" s="5" t="s">
         <v>9</v>
       </c>
@@ -1619,9 +1619,9 @@
         <v>442736</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="43"/>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A15" s="41"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="4" t="s">
         <v>3</v>
       </c>
@@ -1647,7 +1647,7 @@
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
       <c r="Y15" s="4"/>
-      <c r="Z15" s="38"/>
+      <c r="Z15" s="39"/>
       <c r="AA15" s="5" t="s">
         <v>3</v>
       </c>
@@ -1673,9 +1673,9 @@
       <c r="AU15" s="9"/>
       <c r="AV15" s="9"/>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A16" s="40"/>
-      <c r="B16" s="43"/>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A16" s="41"/>
+      <c r="B16" s="44"/>
       <c r="C16" s="4" t="s">
         <v>5</v>
       </c>
@@ -1701,7 +1701,7 @@
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
       <c r="Y16" s="4"/>
-      <c r="Z16" s="38"/>
+      <c r="Z16" s="39"/>
       <c r="AA16" s="5" t="s">
         <v>5</v>
       </c>
@@ -1727,9 +1727,9 @@
       <c r="AU16" s="9"/>
       <c r="AV16" s="9"/>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A17" s="40"/>
-      <c r="B17" s="43"/>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A17" s="41"/>
+      <c r="B17" s="44"/>
       <c r="C17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1755,7 +1755,7 @@
       <c r="W17" s="7"/>
       <c r="X17" s="7"/>
       <c r="Y17" s="4"/>
-      <c r="Z17" s="38"/>
+      <c r="Z17" s="39"/>
       <c r="AA17" s="5" t="s">
         <v>4</v>
       </c>
@@ -1781,9 +1781,9 @@
       <c r="AU17" s="9"/>
       <c r="AV17" s="9"/>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
-      <c r="B18" s="43"/>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A18" s="41"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="4" t="s">
         <v>6</v>
       </c>
@@ -1809,7 +1809,7 @@
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
       <c r="Y18" s="4"/>
-      <c r="Z18" s="38"/>
+      <c r="Z18" s="39"/>
       <c r="AA18" s="5" t="s">
         <v>6</v>
       </c>
@@ -1835,8 +1835,8 @@
       <c r="AU18" s="9"/>
       <c r="AV18" s="9"/>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A19" s="41"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1885,8 +1885,8 @@
       <c r="AU19" s="5"/>
       <c r="AV19" s="5"/>
     </row>
-    <row r="20" spans="1:48" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40"/>
+    <row r="20" spans="1:48" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="41"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1911,7 +1911,7 @@
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
-      <c r="Z20" s="38" t="s">
+      <c r="Z20" s="39" t="s">
         <v>15</v>
       </c>
       <c r="AA20" s="5" t="s">
@@ -2002,9 +2002,9 @@
         <v>2944</v>
       </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="43" t="s">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A21" s="41"/>
+      <c r="B21" s="44" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -2095,7 +2095,7 @@
         <v>17739</v>
       </c>
       <c r="Y21" s="4"/>
-      <c r="Z21" s="38"/>
+      <c r="Z21" s="39"/>
       <c r="AA21" s="5" t="s">
         <v>9</v>
       </c>
@@ -2184,9 +2184,9 @@
         <v>106839</v>
       </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
-      <c r="B22" s="43"/>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A22" s="41"/>
+      <c r="B22" s="44"/>
       <c r="C22" s="4" t="s">
         <v>3</v>
       </c>
@@ -2212,7 +2212,7 @@
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
       <c r="Y22" s="4"/>
-      <c r="Z22" s="38"/>
+      <c r="Z22" s="39"/>
       <c r="AA22" s="5" t="s">
         <v>3</v>
       </c>
@@ -2238,9 +2238,9 @@
       <c r="AU22" s="9"/>
       <c r="AV22" s="9"/>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
-      <c r="B23" s="43"/>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A23" s="41"/>
+      <c r="B23" s="44"/>
       <c r="C23" s="4" t="s">
         <v>5</v>
       </c>
@@ -2266,7 +2266,7 @@
       <c r="W23" s="7"/>
       <c r="X23" s="7"/>
       <c r="Y23" s="4"/>
-      <c r="Z23" s="38"/>
+      <c r="Z23" s="39"/>
       <c r="AA23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2292,9 +2292,9 @@
       <c r="AU23" s="9"/>
       <c r="AV23" s="9"/>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A24" s="40"/>
-      <c r="B24" s="43"/>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A24" s="41"/>
+      <c r="B24" s="44"/>
       <c r="C24" s="4" t="s">
         <v>4</v>
       </c>
@@ -2320,7 +2320,7 @@
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
       <c r="Y24" s="4"/>
-      <c r="Z24" s="38"/>
+      <c r="Z24" s="39"/>
       <c r="AA24" s="5" t="s">
         <v>4</v>
       </c>
@@ -2346,9 +2346,9 @@
       <c r="AU24" s="9"/>
       <c r="AV24" s="9"/>
     </row>
-    <row r="25" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="41"/>
-      <c r="B25" s="44"/>
+    <row r="25" spans="1:48" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="29" t="s">
         <v>6</v>
       </c>
@@ -2374,7 +2374,7 @@
       <c r="W25" s="30"/>
       <c r="X25" s="30"/>
       <c r="Y25" s="29"/>
-      <c r="Z25" s="39"/>
+      <c r="Z25" s="40"/>
       <c r="AA25" s="31" t="s">
         <v>6</v>
       </c>
@@ -2400,7 +2400,7 @@
       <c r="AU25" s="32"/>
       <c r="AV25" s="32"/>
     </row>
-    <row r="26" spans="1:48" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:48" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
       <c r="B26" s="33"/>
       <c r="C26" s="33"/>
@@ -2450,7 +2450,7 @@
       <c r="AU26" s="33"/>
       <c r="AV26" s="33"/>
     </row>
-    <row r="27" spans="1:48" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:48" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" s="34"/>
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
@@ -2516,8 +2516,8 @@
       </c>
       <c r="AV27" s="36"/>
     </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A28" s="42" t="s">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A28" s="43" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="34"/>
@@ -2636,8 +2636,8 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="29" spans="1:48" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="42"/>
+    <row r="29" spans="1:48" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="43"/>
       <c r="B29" s="34"/>
       <c r="C29" s="34" t="s">
         <v>1</v>
@@ -2803,8 +2803,8 @@
         <v>1305600</v>
       </c>
     </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A30" s="42"/>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A30" s="43"/>
       <c r="B30" s="34"/>
       <c r="C30" s="34" t="s">
         <v>3</v>
@@ -2857,8 +2857,8 @@
       <c r="AU30" s="37"/>
       <c r="AV30" s="37"/>
     </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A31" s="43"/>
       <c r="B31" s="34"/>
       <c r="C31" s="34" t="s">
         <v>5</v>
@@ -2911,8 +2911,8 @@
       <c r="AU31" s="37"/>
       <c r="AV31" s="37"/>
     </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A32" s="42"/>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A32" s="43"/>
       <c r="B32" s="34"/>
       <c r="C32" s="34" t="s">
         <v>4</v>
@@ -2965,8 +2965,8 @@
       <c r="AU32" s="37"/>
       <c r="AV32" s="37"/>
     </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A33" s="42"/>
+    <row r="33" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A33" s="43"/>
       <c r="B33" s="34"/>
       <c r="C33" s="34" t="s">
         <v>6</v>

</xml_diff>